<commit_message>
+) Measurements from 06.07.23
</commit_message>
<xml_diff>
--- a/Messungen.xlsx
+++ b/Messungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagib\PycharmProjects\Projektarbeit_Neutronenradiographie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A5C2E6-8881-4624-90F2-95DECECDDE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD86287-CC73-4F8F-A21F-F5F79E31EAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -87,14 +87,23 @@
   <si>
     <t>Nd/No in ‰</t>
   </si>
+  <si>
+    <t>Bemerkung</t>
+  </si>
+  <si>
+    <t>Scan Fehlermeldung beim ersten Versuch: Selected sensitivity is not available.</t>
+  </si>
+  <si>
+    <t>Wiederholungsscan aufgrund der geringen Zählrate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="hh:mm&quot; Uhr&quot;;@"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="hh:mm&quot; Uhr&quot;;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -119,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -207,53 +216,46 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,509 +552,597 @@
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="9" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="18"/>
-    </row>
-    <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="18"/>
+    </row>
+    <row r="2" spans="1:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="Q2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="R2" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>45111</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>0.54722222222222217</v>
       </c>
-      <c r="C3" s="6">
-        <v>60</v>
-      </c>
-      <c r="D3" s="6">
-        <v>60</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="C3">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="11">
         <v>18463</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="11">
         <v>98</v>
       </c>
-      <c r="H3" s="13">
-        <f>IF(N3="","",O3/N3*1000)</f>
+      <c r="H3" s="14">
+        <f>IF(O3="","",P3/O3*1000)</f>
         <v>8.6031554065197078</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="10"/>
+      <c r="J3" s="16">
         <v>45111</v>
       </c>
-      <c r="J3" s="11">
+      <c r="K3" s="8">
         <v>0.59305555555555556</v>
       </c>
-      <c r="K3" s="6">
-        <v>60</v>
-      </c>
-      <c r="L3" s="6">
-        <v>60</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="L3">
+        <v>60</v>
+      </c>
+      <c r="M3">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="15">
+      <c r="O3" s="11">
         <v>36382</v>
       </c>
-      <c r="O3" s="15">
+      <c r="P3" s="11">
         <v>313</v>
       </c>
-      <c r="P3" s="13">
-        <f>IF(N3="","",O3/N3*1000)</f>
+      <c r="Q3" s="14">
+        <f>IF(O3="","",P3/O3*1000)</f>
         <v>8.6031554065197078</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="R3" s="18"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>45112</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C4" s="6">
-        <v>60</v>
-      </c>
-      <c r="D4" s="6">
-        <v>60</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="11">
         <v>1065</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="11">
         <v>10</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="14">
         <f t="shared" ref="H4:H15" si="0">IF(F4="","",G4/F4*1000)</f>
         <v>9.3896713615023479</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="10"/>
+      <c r="J4" s="16">
         <v>45112</v>
       </c>
-      <c r="J4" s="11">
+      <c r="K4" s="8">
         <v>0.47361111111111115</v>
       </c>
-      <c r="K4" s="6">
-        <v>60</v>
-      </c>
-      <c r="L4" s="6">
-        <v>60</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="L4">
+        <v>60</v>
+      </c>
+      <c r="M4">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="15">
+      <c r="O4" s="11">
         <v>23382</v>
       </c>
-      <c r="O4" s="15">
+      <c r="P4" s="11">
         <v>178</v>
       </c>
-      <c r="P4" s="13">
-        <f t="shared" ref="P4:P15" si="1">IF(N4="","",O4/N4*1000)</f>
+      <c r="Q4" s="14">
+        <f t="shared" ref="Q4:Q15" si="1">IF(O4="","",P4/O4*1000)</f>
         <v>7.61269352493371</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="R4" s="18"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>45112</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>0.51874999999999993</v>
       </c>
-      <c r="C5" s="6">
-        <v>60</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
         <v>50</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <v>35708</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="11">
         <v>316</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="14">
         <f t="shared" si="0"/>
         <v>8.8495575221238933</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="10"/>
+      <c r="J5" s="16">
         <v>45113</v>
       </c>
-      <c r="J5" s="11">
+      <c r="K5" s="8">
         <v>0.38541666666666669</v>
       </c>
-      <c r="K5" s="6">
-        <v>60</v>
-      </c>
-      <c r="L5" s="6">
+      <c r="L5">
+        <v>60</v>
+      </c>
+      <c r="M5">
         <v>120</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="13" t="str">
+      <c r="O5" s="11">
+        <v>23299</v>
+      </c>
+      <c r="P5" s="11">
+        <v>189</v>
+      </c>
+      <c r="Q5" s="14">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="13" t="str">
+        <v>8.1119361345980519</v>
+      </c>
+      <c r="R5" s="18"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>45113</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="11">
+        <v>78</v>
+      </c>
+      <c r="G6" s="11">
+        <v>3</v>
+      </c>
+      <c r="H6" s="14">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="13" t="str">
+        <v>38.461538461538467</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="16">
+        <v>45113</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="L6">
+        <v>60</v>
+      </c>
+      <c r="M6">
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="11">
+        <v>33300</v>
+      </c>
+      <c r="P6" s="11">
+        <v>266</v>
+      </c>
+      <c r="Q6" s="14">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="13" t="str">
+        <v>7.9879879879879887</v>
+      </c>
+      <c r="R6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>45113</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="11">
+        <v>71</v>
+      </c>
+      <c r="G7" s="11">
+        <v>3</v>
+      </c>
+      <c r="H7" s="14">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="13" t="str">
+        <v>42.25352112676056</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="16">
+        <v>45113</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="L7">
+        <v>60</v>
+      </c>
+      <c r="M7">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="11">
+        <v>33098</v>
+      </c>
+      <c r="P7" s="11">
+        <v>300</v>
+      </c>
+      <c r="Q7" s="14">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="13" t="str">
+        <v>9.0639917819807838</v>
+      </c>
+      <c r="R7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>45113</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="11">
+        <v>29714</v>
+      </c>
+      <c r="G8" s="11">
+        <v>265</v>
+      </c>
+      <c r="H8" s="14">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="13" t="str">
+        <v>8.9183549841825407</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="8"/>
+      <c r="M8">
+        <v>60</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="13" t="str">
+      <c r="R8" s="18"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="8"/>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="13" t="str">
+      <c r="I9" s="10"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="8"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13" t="str">
+      <c r="R9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="13" t="str">
+      <c r="I10" s="10"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="8"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="13" t="str">
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="8"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="13" t="str">
+      <c r="I11" s="10"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="8"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="13" t="str">
+      <c r="R11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="13" t="str">
+      <c r="I12" s="10"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="8"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="13" t="str">
+      <c r="R12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="13" t="str">
+      <c r="I13" s="10"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="8"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="13" t="str">
+      <c r="R13" s="18"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="8"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="13" t="str">
+      <c r="I14" s="10"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="8"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17" t="str">
+      <c r="R14" s="18"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="17" t="str">
+      <c r="I15" s="13"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="11"/>
+      <c r="R15" s="19"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="J1:Q1"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E15 M3:M15" xr:uid="{59FFFC92-7BED-4CED-BC4B-8EB49C9E10CF}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N15 E3:E15" xr:uid="{59FFFC92-7BED-4CED-BC4B-8EB49C9E10CF}">
       <formula1>"ja,nein"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
+) measurements from 07.07.23
</commit_message>
<xml_diff>
--- a/Messungen.xlsx
+++ b/Messungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagib\PycharmProjects\Projektarbeit_Neutronenradiographie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD86287-CC73-4F8F-A21F-F5F79E31EAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2AD86-8296-40DF-A91B-8C6770B1ADF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -541,7 +541,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,60 +945,119 @@
         <v>8.9183549841825407</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="8"/>
+      <c r="J8" s="16">
+        <v>45114</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="L8">
+        <v>62</v>
+      </c>
       <c r="M8">
         <v>60</v>
       </c>
       <c r="N8" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="14" t="str">
+      <c r="O8" s="11">
+        <v>39325</v>
+      </c>
+      <c r="P8" s="11">
+        <v>341</v>
+      </c>
+      <c r="Q8" s="14">
         <f t="shared" si="1"/>
-        <v/>
+        <v>8.6713286713286717</v>
       </c>
       <c r="R8" s="18"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="4">
+        <v>45114</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
       <c r="D9">
         <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="14" t="str">
+      <c r="F9" s="11">
+        <v>25512</v>
+      </c>
+      <c r="G9" s="11">
+        <v>217</v>
+      </c>
+      <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v/>
+        <v>8.5058011915961114</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="8"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="14" t="str">
+      <c r="J9" s="16">
+        <v>45114</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.52708333333333335</v>
+      </c>
+      <c r="L9">
+        <v>60</v>
+      </c>
+      <c r="M9">
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="11">
+        <v>35261</v>
+      </c>
+      <c r="P9" s="11">
+        <v>294</v>
+      </c>
+      <c r="Q9" s="14">
         <f t="shared" si="1"/>
-        <v/>
+        <v>8.3378236578656306</v>
       </c>
       <c r="R9" s="18"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="8"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14" t="str">
+      <c r="A10" s="4">
+        <v>45114</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="11">
+        <v>39220</v>
+      </c>
+      <c r="G10" s="11">
+        <v>364</v>
+      </c>
+      <c r="H10" s="14">
         <f t="shared" si="0"/>
-        <v/>
+        <v>9.2809790922998463</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="16"/>
       <c r="K10" s="8"/>
+      <c r="M10">
+        <v>120</v>
+      </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="14" t="str">
@@ -1008,13 +1067,30 @@
       <c r="R10" s="18"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14" t="str">
+      <c r="A11" s="4">
+        <v>45114</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="11">
+        <v>23565</v>
+      </c>
+      <c r="G11" s="11">
+        <v>217</v>
+      </c>
+      <c r="H11" s="14">
         <f t="shared" si="0"/>
-        <v/>
+        <v>9.2085720347973705</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="16"/>

</xml_diff>